<commit_message>
new json file and html files for charts and map
</commit_message>
<xml_diff>
--- a/forecast (1).xlsx
+++ b/forecast (1).xlsx
@@ -225,19 +225,19 @@
     <t>Tuyên Quang</t>
   </si>
   <si>
-    <t>Đòng Tháp</t>
-  </si>
-  <si>
     <t>Hưng Yên</t>
   </si>
   <si>
     <t>Vĩnh Long</t>
   </si>
   <si>
-    <t>Huế</t>
-  </si>
-  <si>
-    <t>TP. Hồ Chí Minh</t>
+    <t>Đồng Tháp</t>
+  </si>
+  <si>
+    <t>Thừa Thiên Huế</t>
+  </si>
+  <si>
+    <t>Hồ Chí Minh</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:E273"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +722,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>13.52201557159424</v>
@@ -875,7 +875,7 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16">
         <v>16.650686264038089</v>
@@ -1198,7 +1198,7 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35">
         <v>11.230575561523439</v>
@@ -1300,7 +1300,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C41">
         <v>14.61581516265869</v>
@@ -1453,7 +1453,7 @@
         <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50">
         <v>19.135629653930661</v>
@@ -1776,7 +1776,7 @@
         <v>40</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C69">
         <v>14.03428745269775</v>
@@ -1878,7 +1878,7 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C75">
         <v>15.045980453491209</v>
@@ -2031,7 +2031,7 @@
         <v>21</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C84">
         <v>20.092939376831051</v>
@@ -2354,7 +2354,7 @@
         <v>40</v>
       </c>
       <c r="B103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C103">
         <v>13.535329818725589</v>
@@ -2456,7 +2456,7 @@
         <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C109">
         <v>13.411045074462891</v>
@@ -2609,7 +2609,7 @@
         <v>21</v>
       </c>
       <c r="B118" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C118">
         <v>19.279018402099609</v>
@@ -2932,7 +2932,7 @@
         <v>40</v>
       </c>
       <c r="B137" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C137">
         <v>12.7104434967041</v>
@@ -3034,7 +3034,7 @@
         <v>10</v>
       </c>
       <c r="B143" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C143">
         <v>13.068874359130859</v>
@@ -3187,7 +3187,7 @@
         <v>21</v>
       </c>
       <c r="B152" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C152">
         <v>20.529621124267582</v>
@@ -3510,7 +3510,7 @@
         <v>40</v>
       </c>
       <c r="B171" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C171">
         <v>12.022871017456049</v>
@@ -3612,7 +3612,7 @@
         <v>10</v>
       </c>
       <c r="B177" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C177">
         <v>11.952693939208981</v>
@@ -3765,7 +3765,7 @@
         <v>21</v>
       </c>
       <c r="B186" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C186">
         <v>19.122869491577148</v>
@@ -4088,7 +4088,7 @@
         <v>40</v>
       </c>
       <c r="B205" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C205">
         <v>11.44509220123291</v>
@@ -4190,7 +4190,7 @@
         <v>10</v>
       </c>
       <c r="B211" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C211">
         <v>14.56663608551025</v>
@@ -4343,7 +4343,7 @@
         <v>21</v>
       </c>
       <c r="B220" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C220">
         <v>19.588014602661129</v>
@@ -4666,7 +4666,7 @@
         <v>40</v>
       </c>
       <c r="B239" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C239">
         <v>13.899361610412599</v>
@@ -4768,7 +4768,7 @@
         <v>10</v>
       </c>
       <c r="B245" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C245">
         <v>13.477962493896481</v>
@@ -4921,7 +4921,7 @@
         <v>21</v>
       </c>
       <c r="B254" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C254">
         <v>21.080097198486332</v>
@@ -5244,7 +5244,7 @@
         <v>40</v>
       </c>
       <c r="B273" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C273">
         <v>12.21780490875244</v>

</xml_diff>